<commit_message>
Zip Breaker 2 updates
</commit_message>
<xml_diff>
--- a/ZipBreakerAkka2/src/test/resources/PerformanceTests.xlsx
+++ b/ZipBreakerAkka2/src/test/resources/PerformanceTests.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="21735" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -24,10 +25,6 @@
   <si>
     <t>Java - Fork Join
 (single JVM)</t>
-  </si>
-  <si>
-    <t>Akka Distributed
-(3 pysical machines)</t>
   </si>
   <si>
     <t>1.000.000 passwords</t>
@@ -101,6 +98,10 @@
   </si>
   <si>
     <t>0 passwords</t>
+  </si>
+  <si>
+    <t>Akka Distributed
+(2 pysical machines)</t>
   </si>
 </sst>
 </file>
@@ -615,15 +616,12 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Processing Time Comparison (1 million passwords)</c:v>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$D$3</c:f>
+              <c:f>Sheet1!$B$3:$E$3</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Classic Java code
 (single threaded)</c:v>
@@ -635,16 +633,20 @@
                 <c:pt idx="2">
                   <c:v>Akka Distributed
 (single physical machine)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Akka Distributed
+(2 pysical machines)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$D$5</c:f>
+              <c:f>Sheet1!$B$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>672857</c:v>
                 </c:pt>
@@ -653,6 +655,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>428763</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185226</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -668,12 +673,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="91588608"/>
-        <c:axId val="60141504"/>
+        <c:axId val="64252416"/>
+        <c:axId val="61892864"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="91588608"/>
+        <c:axId val="64252416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -682,7 +687,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60141504"/>
+        <c:crossAx val="61892864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -690,7 +695,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60141504"/>
+        <c:axId val="61892864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,7 +706,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91588608"/>
+        <c:crossAx val="64252416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -939,6 +944,73 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Akka Distributed
+(2 pysical machines)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$4:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0 passwords</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.000.000 passwords</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.000.000 passwords</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.000.000 passwords</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.000.000 passwords</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>185226</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>370398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>556172</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>741398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -949,11 +1021,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95003648"/>
-        <c:axId val="96051200"/>
+        <c:axId val="64253440"/>
+        <c:axId val="61894016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95003648"/>
+        <c:axId val="64253440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -962,7 +1034,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96051200"/>
+        <c:crossAx val="61894016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -970,7 +1042,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96051200"/>
+        <c:axId val="61894016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,7 +1053,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95003648"/>
+        <c:crossAx val="64253440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1358,7 +1430,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A2" activeCellId="1" sqref="A2:E2 A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,7 +1444,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="144" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -1381,7 +1453,7 @@
     </row>
     <row r="2" spans="1:5" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1397,15 +1469,15 @@
         <v>1</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="7">
         <v>4</v>
@@ -1422,7 +1494,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="7">
         <v>672857</v>
@@ -1433,11 +1505,13 @@
       <c r="D5" s="17">
         <v>428763</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="6">
+        <v>185226</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="8">
         <v>1384675</v>
@@ -1448,11 +1522,13 @@
       <c r="D6" s="18">
         <v>867263</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>370398</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="8">
         <v>2038052</v>
@@ -1463,11 +1539,13 @@
       <c r="D7" s="18">
         <v>1295277</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <v>556172</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="9">
         <v>2686690</v>
@@ -1478,7 +1556,9 @@
       <c r="D8" s="19">
         <v>1728837</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4">
+        <v>741398</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>